<commit_message>
Baby model done plus some papers
</commit_message>
<xml_diff>
--- a/Code/Data/Monthly.xlsx
+++ b/Code/Data/Monthly.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly" sheetId="1" r:id="rId1"/>
@@ -1452,10 +1452,10 @@
   <dimension ref="A1:AH837"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="O818" sqref="O818"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>